<commit_message>
descw-1247 finishing touches on model/view
* add generic controller tempmlate
* finish model
* finish styling and carbone templating on view
* fixed some linter errors in `useController`
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_20_rpt_PA_Billed.xlsx
+++ b/backend/reports/xlsx/Tab_20_rpt_PA_Billed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{862AB741-6B43-B743-A274-E9D009B1BE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E8918C-017D-E749-B885-3EBA3F620E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,116 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>{$r1.portfolio_name}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>TOTAL:</t>
   </si>
   <si>
-    <t>Total Recoveries For Projects</t>
-  </si>
-  <si>
-    <t>Less All Project Expenses</t>
-  </si>
-  <si>
-    <t>Q1 Gross Recoveries</t>
-  </si>
-  <si>
-    <t>Q1 Net Recoveries</t>
-  </si>
-  <si>
-    <t>Q2 Gross Recoveries</t>
-  </si>
-  <si>
-    <t>Q2 Net Recoveries</t>
-  </si>
-  <si>
-    <t>Q3 Gross Recoveries</t>
-  </si>
-  <si>
-    <t>Q3 Net Recoveries</t>
-  </si>
-  <si>
-    <t>Q4 Gross Recoveries</t>
-  </si>
-  <si>
-    <t>Q4 Net Recoveries</t>
-  </si>
-  <si>
-    <t>Net Recoveries</t>
-  </si>
-  <si>
-    <t>{$r.total_recoveries}</t>
-  </si>
-  <si>
-    <t>{$r.less_all_project_expenses}</t>
-  </si>
-  <si>
-    <t>{$r.net_recoveries}</t>
-  </si>
-  <si>
-    <t>{$r.q1_gross}</t>
-  </si>
-  <si>
-    <t>{$r.q1_net}</t>
-  </si>
-  <si>
-    <t>{$r.q2_gross}</t>
-  </si>
-  <si>
-    <t>{$r.q2_net}</t>
-  </si>
-  <si>
-    <t>{$r.q3_gross}</t>
-  </si>
-  <si>
-    <t>{$r.q3_net}</t>
-  </si>
-  <si>
-    <t>{$r.q4_gross}</t>
-  </si>
-  <si>
-    <t>{$r.q4_net}</t>
-  </si>
-  <si>
-    <t>{$t.totals_recoveries}</t>
-  </si>
-  <si>
-    <t>{$t.totals_less_all_project_expenses}</t>
-  </si>
-  <si>
-    <t>{$t.totals_net_recoveries}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q1_gross}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q1_net}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q2_gross}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q2_net}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q3_gross}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q3_net}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q4_gross}</t>
-  </si>
-  <si>
-    <t>{$t.totals_q4_net}</t>
-  </si>
-  <si>
-    <t>{$r.portfolio_name}</t>
-  </si>
-  <si>
     <t>{#r=d.report[i]}</t>
   </si>
   <si>
@@ -155,16 +50,73 @@
     <t>{#t=d.report_totals[i]}</t>
   </si>
   <si>
-    <t>{#fy=d.fiscal}</t>
-  </si>
-  <si>
     <t>{#date=d.date}</t>
   </si>
   <si>
-    <t>Net Recovery Summary By Quarter for Fiscal Year {$fy}</t>
-  </si>
-  <si>
-    <t>Portfolios</t>
+    <t>Project JVs Processed for Fiscal {$fy} as of {$date}</t>
+  </si>
+  <si>
+    <t>Project #</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>{$r.project_number}</t>
+  </si>
+  <si>
+    <t>{$r1.project_number}</t>
+  </si>
+  <si>
+    <t>{$r.project_name}</t>
+  </si>
+  <si>
+    <t>{$r.q1}</t>
+  </si>
+  <si>
+    <t>{$r.q2}</t>
+  </si>
+  <si>
+    <t>{$r.q3}</t>
+  </si>
+  <si>
+    <t>{$r.q4}</t>
+  </si>
+  <si>
+    <t>{$r.q_total}</t>
+  </si>
+  <si>
+    <t>{$t.q1_total}</t>
+  </si>
+  <si>
+    <t>{$t.grand_total}</t>
+  </si>
+  <si>
+    <t>{$t.q3_total}</t>
+  </si>
+  <si>
+    <t>{$t.q4_total}</t>
+  </si>
+  <si>
+    <t>{$t.q2_total}</t>
+  </si>
+  <si>
+    <t>{#fy=d.fiscal_year}</t>
   </si>
 </sst>
 </file>
@@ -206,8 +158,8 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="8.5"/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -220,13 +172,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FF003365"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF003365"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,54 +258,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,7 +330,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>32837</xdr:colOff>
+      <xdr:colOff>1561691</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -421,7 +362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2412174" cy="680356"/>
+          <a:ext cx="2411054" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -730,205 +671,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}">
-  <dimension ref="A1:L11"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;Lrpt_PF_NetRecoverySummaryByQuarter&amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>
   </headerFooter>

</xml_diff>